<commit_message>
Added Extra difficulty ACE: Fixed bug when copying and pasting Hold notes ACE: Added Rotate 90 degrees and Expand Medium to Hard transform options Difficulty list is now sorted on Song Select screen Added Section markers to note highways (gameplay and editor)
</commit_message>
<xml_diff>
--- a/Docs/Editor Controls.xlsx
+++ b/Docs/Editor Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sgtbash\Unity Projects\BandBoomBox\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12C1001-059A-4977-8B7D-F784F104E70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC74F14-AB67-4531-937E-A443E6CB4A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="3285" windowWidth="28800" windowHeight="15435" xr2:uid="{8FAE3995-B756-45C1-992C-7EDA11427471}"/>
+    <workbookView xWindow="38400" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{8FAE3995-B756-45C1-992C-7EDA11427471}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Left / Right</t>
   </si>
@@ -142,10 +142,13 @@
     <t>(During playback) Stop - return to playback start</t>
   </si>
   <si>
-    <t>Ctrl + S</t>
-  </si>
-  <si>
     <t>Save</t>
+  </si>
+  <si>
+    <t>Swap hands (for notes at current position)</t>
+  </si>
+  <si>
+    <t>Play From Beginning</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C78DA6-D9EA-4F88-913E-4FD1D4429592}">
-  <dimension ref="A2:B28"/>
+  <dimension ref="A2:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,68 +615,84 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
+      <c r="A18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>